<commit_message>
fix: template fichier xlsx (850)
</commit_message>
<xml_diff>
--- a/public/model/template_import_PILOTE.xlsx
+++ b/public/model/template_import_PILOTE.xlsx
@@ -1,35 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkervella-adc\Desktop\Pilote 2\Indicateurs\module_import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lchareyron-adc\Desktop\Fichiers correctifs datafactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3A35AA-A6BE-4A41-BF63-68BFD5A10CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{44FF8DC4-34E1-4F71-ADE9-02E30B4C48C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>KERVELLA Gaelle</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5A9524B4-838C-427A-9428-9E9E2DCFED9E}">
       <text>
         <r>
           <rPr>
@@ -60,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{45182F93-3758-46B0-81F4-5C7C8FC300E8}">
       <text>
         <r>
           <rPr>
@@ -103,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{4C1003C3-13FF-4FCD-B141-B943955B6D23}">
       <text>
         <r>
           <rPr>
@@ -132,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{3EB806A9-53D9-4CE5-8275-E87F50AD763E}">
       <text>
         <r>
           <rPr>
@@ -145,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{01034BB9-23C2-4B43-BD01-4544CD7FCC80}">
       <text>
         <r>
           <rPr>
@@ -160,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{83DEA9A6-2F29-4D97-BBC9-C20C7D5EF7B5}">
       <text>
         <r>
           <rPr>
@@ -196,6 +206,9 @@
     <t>zone_id</t>
   </si>
   <si>
+    <t>zone_nom</t>
+  </si>
+  <si>
     <t>date_valeur</t>
   </si>
   <si>
@@ -204,21 +217,18 @@
   <si>
     <t>valeur</t>
   </si>
-  <si>
-    <t>zone_nom</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
@@ -265,83 +275,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFD0CECE"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -370,7 +311,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -382,7 +323,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -399,9 +340,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -429,14 +370,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -464,6 +422,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -615,20 +590,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABAA8EC-0665-49A0-AE44-AF0B2EAEEC25}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -638,25 +607,20 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>